<commit_message>
Correcting the final model outputs to add binary predictions
</commit_message>
<xml_diff>
--- a/Modelos_finales_y_entregable/models_outputs.xlsx
+++ b/Modelos_finales_y_entregable/models_outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmeji\Documents\EAFIT\MasterDataScience\EC1209_Metodos_Avanzados_Estadistica\competencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C465ADA7-C915-4E52-9D53-A79840E39C54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB68C5B-6145-4872-B2E8-E4FB7CE539CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{CD350190-85C6-4B02-820A-A669D59AA316}"/>
   </bookViews>
@@ -31,15 +31,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Output Cont.</t>
   </si>
   <si>
-    <t>Output Bin.</t>
+    <t>Output Count.</t>
   </si>
   <si>
-    <t>Output Count.</t>
+    <t>Output Binary Predict Probability</t>
+  </si>
+  <si>
+    <t>Output Binary Prediction</t>
   </si>
 </sst>
 </file>
@@ -391,15 +394,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690664D7-9110-4CCC-9A4A-D1B7EA1299E4}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A26"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,280 +418,358 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.46139728520215001</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>0.77833636687316499</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.06132039054129</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>0.82976889821486699</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.0604678660928202</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>0.93556838370242301</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.98496149696976</v>
       </c>
       <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>0.92592281336670601</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-0.72196094129164201</v>
       </c>
       <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>0.45768622345343501</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.236637976713061</v>
       </c>
       <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>0.22484349031918699</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-0.29900546769751002</v>
       </c>
       <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
         <v>0.30016175333738998</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-0.74829881821663402</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>0.39656633209367897</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-1.93955721589703</v>
       </c>
       <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
         <v>0.61946375140446297</v>
       </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2.9548584251357601</v>
       </c>
       <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
         <v>0.70597896121883896</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2.3542202686213201</v>
       </c>
       <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>0.94251458651727205</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2.1510595382669502</v>
       </c>
       <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
         <v>0.925800400267073</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-0.53225125566426001</v>
       </c>
       <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
         <v>0.41423885104748398</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-0.56948996672922003</v>
       </c>
       <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
         <v>0.80404109061388296</v>
       </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.1709003244528602</v>
       </c>
       <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
         <v>0.93200782269657101</v>
       </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-0.33452788818505202</v>
       </c>
       <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
         <v>0.84690434108880497</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.18727967918640001</v>
       </c>
       <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
         <v>0.48881517971375499</v>
       </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.69935103090956496</v>
       </c>
       <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
         <v>0.77473755754008899</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2.2491174464699402</v>
       </c>
       <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
         <v>0.93044020964600305</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.2710068639118099</v>
       </c>
       <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
         <v>0.77184994876995805</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.84153661187883599</v>
       </c>
       <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
         <v>0.77637663068700602</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.66512958368882802</v>
       </c>
       <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
         <v>0.68603308015003595</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2.1586953380571101</v>
       </c>
       <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
         <v>0.93762713271014297</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-1.4416107127398201</v>
       </c>
       <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
         <v>0.34190422099310103</v>
       </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-0.68018889671248595</v>
       </c>
       <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
         <v>0.348880637928426</v>
       </c>
-      <c r="C26">
-        <v>2</v>
+      <c r="D26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>